<commit_message>
This is my 5th commit message
</commit_message>
<xml_diff>
--- a/testData/Magento_LoginData.xlsx
+++ b/testData/Magento_LoginData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://staffingaditi-my.sharepoint.com/personal/ranjithas_aditiconsulting_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranjithas\advance-selenium\Magento\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{1EC9806D-2BDD-4ADD-B48C-134444DB788B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90F81F79-8A8A-46CE-9088-EB18FE6DEDDE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF25DAA3-A3C4-4AA3-8D00-64A3273458A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1044" yWindow="1044" windowWidth="7500" windowHeight="6000" xr2:uid="{FC12888A-A085-4C4C-B81C-96AC5F3E51A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FC12888A-A085-4C4C-B81C-96AC5F3E51A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">                Password</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Valid</t>
+  </si>
+  <si>
+    <t>test@9162123</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +518,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>

</xml_diff>